<commit_message>
Fix #5457 EMX missing required label attribute errors Fix emx_deep_nesting.xlsx resource: make extended entity abstract
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/xls/emx_deep_nesting.xlsx
+++ b/molgenis-app/src/test/resources/xls/emx_deep_nesting.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="160" windowWidth="33600" windowHeight="20480" tabRatio="686" activeTab="2"/>
+    <workbookView xWindow="3240" yWindow="165" windowWidth="29040" windowHeight="16440" tabRatio="686" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="1" r:id="rId1"/>
@@ -1697,6 +1697,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2028,13 +2033,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2045,7 +2050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2053,7 +2058,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>344</v>
       </c>
@@ -2079,13 +2084,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2102,7 +2111,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2110,18 +2119,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
       <c r="E3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2132,22 +2144,22 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -2167,19 +2179,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2208,7 +2221,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2222,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2239,7 +2252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2256,7 +2269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2276,7 +2289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>132</v>
       </c>
@@ -2296,7 +2309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>139</v>
       </c>
@@ -2313,7 +2326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>133</v>
       </c>
@@ -2333,7 +2346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>396</v>
       </c>
@@ -2350,7 +2363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>397</v>
       </c>
@@ -2373,7 +2386,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>398</v>
       </c>
@@ -2393,7 +2406,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -2410,7 +2423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2427,7 +2440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2441,7 +2454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2458,7 +2471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>138</v>
       </c>
@@ -2478,7 +2491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2492,7 +2505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>241</v>
       </c>
@@ -2512,7 +2525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>343</v>
       </c>
@@ -2529,7 +2542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2546,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>242</v>
       </c>
@@ -2585,13 +2598,13 @@
       <selection activeCell="F2" sqref="F2:F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -2611,7 +2624,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>243</v>
       </c>
@@ -2631,7 +2644,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>244</v>
       </c>
@@ -2651,7 +2664,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>245</v>
       </c>
@@ -2671,7 +2684,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>246</v>
       </c>
@@ -2691,7 +2704,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -2711,7 +2724,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>248</v>
       </c>
@@ -2731,7 +2744,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>249</v>
       </c>
@@ -2751,7 +2764,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>250</v>
       </c>
@@ -2771,7 +2784,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>251</v>
       </c>
@@ -2791,7 +2804,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>252</v>
       </c>
@@ -2811,7 +2824,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>253</v>
       </c>
@@ -2831,7 +2844,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>254</v>
       </c>
@@ -2851,7 +2864,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>255</v>
       </c>
@@ -2871,7 +2884,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>256</v>
       </c>
@@ -2891,7 +2904,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>257</v>
       </c>
@@ -2911,7 +2924,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>258</v>
       </c>
@@ -2931,7 +2944,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>259</v>
       </c>
@@ -2951,7 +2964,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>260</v>
       </c>
@@ -2971,7 +2984,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>261</v>
       </c>
@@ -2991,7 +3004,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>262</v>
       </c>
@@ -3011,7 +3024,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>263</v>
       </c>
@@ -3031,7 +3044,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>264</v>
       </c>
@@ -3051,7 +3064,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>265</v>
       </c>
@@ -3071,7 +3084,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>266</v>
       </c>
@@ -3091,7 +3104,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>267</v>
       </c>
@@ -3111,7 +3124,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>268</v>
       </c>
@@ -3131,7 +3144,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>269</v>
       </c>
@@ -3151,7 +3164,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>270</v>
       </c>
@@ -3171,7 +3184,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>271</v>
       </c>
@@ -3191,7 +3204,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>272</v>
       </c>
@@ -3211,7 +3224,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>273</v>
       </c>
@@ -3231,7 +3244,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>274</v>
       </c>
@@ -3251,7 +3264,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>275</v>
       </c>
@@ -3271,7 +3284,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>276</v>
       </c>
@@ -3291,7 +3304,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>277</v>
       </c>
@@ -3311,7 +3324,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>278</v>
       </c>
@@ -3331,7 +3344,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>279</v>
       </c>
@@ -3351,7 +3364,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>280</v>
       </c>
@@ -3371,7 +3384,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>281</v>
       </c>
@@ -3391,7 +3404,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>282</v>
       </c>
@@ -3411,7 +3424,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>283</v>
       </c>
@@ -3431,7 +3444,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>284</v>
       </c>
@@ -3451,7 +3464,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>285</v>
       </c>
@@ -3471,7 +3484,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>286</v>
       </c>
@@ -3491,7 +3504,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>287</v>
       </c>
@@ -3511,7 +3524,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>288</v>
       </c>
@@ -3531,7 +3544,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>289</v>
       </c>
@@ -3551,7 +3564,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>290</v>
       </c>
@@ -3571,7 +3584,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>291</v>
       </c>
@@ -3591,7 +3604,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>292</v>
       </c>
@@ -3630,15 +3643,15 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.875" customWidth="1"/>
+    <col min="8" max="8" width="21.625" customWidth="1"/>
     <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -3667,7 +3680,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>345</v>
       </c>
@@ -3696,7 +3709,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>346</v>
       </c>
@@ -3725,7 +3738,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>347</v>
       </c>
@@ -3754,7 +3767,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>348</v>
       </c>
@@ -3783,7 +3796,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>349</v>
       </c>
@@ -3812,7 +3825,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>350</v>
       </c>
@@ -3841,7 +3854,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>351</v>
       </c>
@@ -3870,7 +3883,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>352</v>
       </c>
@@ -3899,7 +3912,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>353</v>
       </c>
@@ -3928,7 +3941,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>354</v>
       </c>
@@ -3957,7 +3970,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>355</v>
       </c>
@@ -3986,7 +3999,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>356</v>
       </c>
@@ -4015,7 +4028,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>357</v>
       </c>
@@ -4044,7 +4057,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>358</v>
       </c>
@@ -4073,7 +4086,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>359</v>
       </c>
@@ -4102,7 +4115,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>360</v>
       </c>
@@ -4131,7 +4144,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>361</v>
       </c>
@@ -4160,7 +4173,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>362</v>
       </c>
@@ -4189,7 +4202,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>363</v>
       </c>
@@ -4218,7 +4231,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>364</v>
       </c>
@@ -4247,7 +4260,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>365</v>
       </c>
@@ -4276,7 +4289,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>366</v>
       </c>
@@ -4305,7 +4318,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>367</v>
       </c>
@@ -4334,7 +4347,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>368</v>
       </c>
@@ -4363,7 +4376,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>369</v>
       </c>
@@ -4392,7 +4405,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>370</v>
       </c>
@@ -4421,7 +4434,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>371</v>
       </c>
@@ -4450,7 +4463,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>372</v>
       </c>
@@ -4479,7 +4492,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>373</v>
       </c>
@@ -4508,7 +4521,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>374</v>
       </c>
@@ -4537,7 +4550,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>375</v>
       </c>
@@ -4566,7 +4579,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>376</v>
       </c>
@@ -4595,7 +4608,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>377</v>
       </c>
@@ -4624,7 +4637,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>378</v>
       </c>
@@ -4653,7 +4666,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>379</v>
       </c>
@@ -4682,7 +4695,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>380</v>
       </c>
@@ -4711,7 +4724,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>381</v>
       </c>
@@ -4740,7 +4753,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>382</v>
       </c>
@@ -4769,7 +4782,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>383</v>
       </c>
@@ -4798,7 +4811,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>384</v>
       </c>
@@ -4827,7 +4840,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>385</v>
       </c>
@@ -4856,7 +4869,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>386</v>
       </c>
@@ -4885,7 +4898,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>387</v>
       </c>
@@ -4914,7 +4927,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>388</v>
       </c>
@@ -4943,7 +4956,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>389</v>
       </c>
@@ -4972,7 +4985,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>390</v>
       </c>
@@ -5001,7 +5014,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>391</v>
       </c>
@@ -5030,7 +5043,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>392</v>
       </c>
@@ -5059,7 +5072,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>393</v>
       </c>
@@ -5088,7 +5101,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>394</v>
       </c>
@@ -5136,12 +5149,12 @@
       <selection activeCell="A2" sqref="A2:A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -5149,7 +5162,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5157,7 +5170,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5165,7 +5178,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5173,7 +5186,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5181,7 +5194,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5189,7 +5202,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5197,7 +5210,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5205,7 +5218,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5213,7 +5226,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5221,7 +5234,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5229,7 +5242,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5237,7 +5250,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5245,7 +5258,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5253,7 +5266,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5261,7 +5274,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5269,7 +5282,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5277,7 +5290,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5285,7 +5298,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5293,7 +5306,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5301,7 +5314,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5309,7 +5322,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5317,7 +5330,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5325,7 +5338,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5333,7 +5346,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5341,7 +5354,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5349,7 +5362,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5357,7 +5370,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5365,7 +5378,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5373,7 +5386,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5381,7 +5394,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5389,7 +5402,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5397,7 +5410,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5405,7 +5418,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5413,7 +5426,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5421,7 +5434,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5429,7 +5442,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5437,7 +5450,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5445,7 +5458,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5453,7 +5466,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5461,7 +5474,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5469,7 +5482,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5477,7 +5490,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5485,7 +5498,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5493,7 +5506,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5501,7 +5514,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5509,7 +5522,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5517,7 +5530,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5525,7 +5538,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5533,7 +5546,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5541,7 +5554,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5568,12 +5581,12 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -5584,7 +5597,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -5595,7 +5608,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -5606,7 +5619,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -5617,7 +5630,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -5628,7 +5641,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -5639,7 +5652,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -5650,7 +5663,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>88</v>
       </c>
@@ -5661,7 +5674,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>89</v>
       </c>
@@ -5672,7 +5685,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -5683,7 +5696,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>91</v>
       </c>
@@ -5694,7 +5707,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>92</v>
       </c>
@@ -5705,7 +5718,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -5716,7 +5729,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -5727,7 +5740,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -5738,7 +5751,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>96</v>
       </c>
@@ -5749,7 +5762,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>97</v>
       </c>
@@ -5760,7 +5773,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>98</v>
       </c>
@@ -5771,7 +5784,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -5782,7 +5795,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -5793,7 +5806,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -5804,7 +5817,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -5815,7 +5828,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -5826,7 +5839,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -5837,7 +5850,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -5848,7 +5861,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>106</v>
       </c>
@@ -5859,7 +5872,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -5870,7 +5883,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -5881,7 +5894,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>109</v>
       </c>
@@ -5892,7 +5905,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>110</v>
       </c>
@@ -5903,7 +5916,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>111</v>
       </c>
@@ -5914,7 +5927,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -5925,7 +5938,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>113</v>
       </c>
@@ -5936,7 +5949,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>114</v>
       </c>
@@ -5947,7 +5960,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>115</v>
       </c>
@@ -5958,7 +5971,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>116</v>
       </c>
@@ -5969,7 +5982,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>117</v>
       </c>
@@ -5980,7 +5993,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>118</v>
       </c>
@@ -5991,7 +6004,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>119</v>
       </c>
@@ -6002,7 +6015,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>120</v>
       </c>
@@ -6013,7 +6026,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>121</v>
       </c>
@@ -6024,7 +6037,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>122</v>
       </c>
@@ -6035,7 +6048,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>123</v>
       </c>
@@ -6046,7 +6059,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>124</v>
       </c>
@@ -6057,7 +6070,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>125</v>
       </c>
@@ -6068,7 +6081,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>126</v>
       </c>
@@ -6079,7 +6092,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>127</v>
       </c>
@@ -6090,7 +6103,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>128</v>
       </c>
@@ -6101,7 +6114,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>129</v>
       </c>
@@ -6112,7 +6125,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>130</v>
       </c>
@@ -6123,7 +6136,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>131</v>
       </c>
@@ -6153,13 +6166,13 @@
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -6170,7 +6183,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -6181,7 +6194,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -6192,7 +6205,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -6203,7 +6216,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>143</v>
       </c>
@@ -6214,7 +6227,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -6225,7 +6238,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>145</v>
       </c>
@@ -6236,7 +6249,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>146</v>
       </c>
@@ -6247,7 +6260,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>147</v>
       </c>
@@ -6258,7 +6271,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>148</v>
       </c>
@@ -6269,7 +6282,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>149</v>
       </c>
@@ -6280,7 +6293,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>150</v>
       </c>
@@ -6291,7 +6304,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>151</v>
       </c>
@@ -6302,7 +6315,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>152</v>
       </c>
@@ -6313,7 +6326,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>153</v>
       </c>
@@ -6324,7 +6337,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>154</v>
       </c>
@@ -6335,7 +6348,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>155</v>
       </c>
@@ -6346,7 +6359,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>156</v>
       </c>
@@ -6357,7 +6370,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>157</v>
       </c>
@@ -6368,7 +6381,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>158</v>
       </c>
@@ -6379,7 +6392,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>159</v>
       </c>
@@ -6390,7 +6403,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>160</v>
       </c>
@@ -6401,7 +6414,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>161</v>
       </c>
@@ -6412,7 +6425,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>162</v>
       </c>
@@ -6423,7 +6436,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>163</v>
       </c>
@@ -6434,7 +6447,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>164</v>
       </c>
@@ -6445,7 +6458,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>165</v>
       </c>
@@ -6456,7 +6469,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>166</v>
       </c>
@@ -6467,7 +6480,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>167</v>
       </c>
@@ -6478,7 +6491,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>168</v>
       </c>
@@ -6489,7 +6502,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>169</v>
       </c>
@@ -6500,7 +6513,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>170</v>
       </c>
@@ -6511,7 +6524,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>171</v>
       </c>
@@ -6522,7 +6535,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>172</v>
       </c>
@@ -6533,7 +6546,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>173</v>
       </c>
@@ -6544,7 +6557,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>174</v>
       </c>
@@ -6555,7 +6568,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>175</v>
       </c>
@@ -6566,7 +6579,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>176</v>
       </c>
@@ -6577,7 +6590,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>177</v>
       </c>
@@ -6588,7 +6601,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>178</v>
       </c>
@@ -6599,7 +6612,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>179</v>
       </c>
@@ -6610,7 +6623,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>180</v>
       </c>
@@ -6621,7 +6634,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>181</v>
       </c>
@@ -6632,7 +6645,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>182</v>
       </c>
@@ -6643,7 +6656,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>183</v>
       </c>
@@ -6654,7 +6667,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>184</v>
       </c>
@@ -6665,7 +6678,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>185</v>
       </c>
@@ -6676,7 +6689,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>186</v>
       </c>
@@ -6687,7 +6700,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>187</v>
       </c>
@@ -6698,7 +6711,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>188</v>
       </c>
@@ -6709,7 +6722,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>189</v>
       </c>
@@ -6739,9 +6752,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -6749,7 +6762,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>190</v>
       </c>
@@ -6757,7 +6770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>191</v>
       </c>
@@ -6765,7 +6778,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>192</v>
       </c>
@@ -6773,7 +6786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>193</v>
       </c>
@@ -6781,7 +6794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>194</v>
       </c>
@@ -6789,7 +6802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>195</v>
       </c>
@@ -6797,7 +6810,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>196</v>
       </c>
@@ -6805,7 +6818,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>197</v>
       </c>
@@ -6813,7 +6826,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>198</v>
       </c>
@@ -6821,7 +6834,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>199</v>
       </c>
@@ -6829,7 +6842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>200</v>
       </c>
@@ -6837,7 +6850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>201</v>
       </c>
@@ -6845,7 +6858,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>202</v>
       </c>
@@ -6853,7 +6866,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>203</v>
       </c>
@@ -6861,7 +6874,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>204</v>
       </c>
@@ -6869,7 +6882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>205</v>
       </c>
@@ -6877,7 +6890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>206</v>
       </c>
@@ -6885,7 +6898,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>207</v>
       </c>
@@ -6893,7 +6906,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>208</v>
       </c>
@@ -6901,7 +6914,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>209</v>
       </c>
@@ -6909,7 +6922,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>210</v>
       </c>
@@ -6917,7 +6930,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>211</v>
       </c>
@@ -6925,7 +6938,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>212</v>
       </c>
@@ -6933,7 +6946,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>213</v>
       </c>
@@ -6941,7 +6954,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>214</v>
       </c>
@@ -6949,7 +6962,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>215</v>
       </c>
@@ -6957,7 +6970,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>216</v>
       </c>
@@ -6965,7 +6978,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>217</v>
       </c>
@@ -6973,7 +6986,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>218</v>
       </c>
@@ -6981,7 +6994,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>219</v>
       </c>
@@ -6989,7 +7002,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>220</v>
       </c>
@@ -6997,7 +7010,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>221</v>
       </c>
@@ -7005,7 +7018,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>222</v>
       </c>
@@ -7013,7 +7026,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>223</v>
       </c>
@@ -7021,7 +7034,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>224</v>
       </c>
@@ -7029,7 +7042,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>225</v>
       </c>
@@ -7037,7 +7050,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>226</v>
       </c>
@@ -7045,7 +7058,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>227</v>
       </c>
@@ -7053,7 +7066,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>228</v>
       </c>
@@ -7061,7 +7074,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>229</v>
       </c>
@@ -7069,7 +7082,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>230</v>
       </c>
@@ -7077,7 +7090,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>231</v>
       </c>
@@ -7085,7 +7098,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>232</v>
       </c>
@@ -7093,7 +7106,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>233</v>
       </c>
@@ -7101,7 +7114,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>234</v>
       </c>
@@ -7109,7 +7122,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>235</v>
       </c>
@@ -7117,7 +7130,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>236</v>
       </c>
@@ -7125,7 +7138,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>237</v>
       </c>
@@ -7133,7 +7146,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>238</v>
       </c>
@@ -7141,7 +7154,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>239</v>
       </c>

</xml_diff>